<commit_message>
created grid templates to print. useful for making planting jigs.
</commit_message>
<xml_diff>
--- a/GH_data/dist_trans_Jan2020.xlsx
+++ b/GH_data/dist_trans_Jan2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisarosenthal/Box/mesocosm expt/mesocosm.git/GH_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6233D7D8-F0B0-9C40-A8F8-D7CD90F49931}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC22459-665C-5A47-81C8-440F18CBD04E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="460" windowWidth="23780" windowHeight="14280" xr2:uid="{7FF54E09-DD73-9C40-B3CF-D76078D6E5CE}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1665" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1670" uniqueCount="36">
   <si>
     <t>tray_1</t>
   </si>
@@ -133,12 +133,27 @@
   <si>
     <t>prim</t>
   </si>
+  <si>
+    <t xml:space="preserve">plants sowed: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">plants inoculated: </t>
+  </si>
+  <si>
+    <t>1/15/20 &amp; 1/17/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inoculum: </t>
+  </si>
+  <si>
+    <t>3 days old</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -155,6 +170,13 @@
     <font>
       <sz val="12"/>
       <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.14999847407452621"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -180,9 +202,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,15 +521,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CA244F-C062-B04D-AD28-1E41D000D4D0}">
-  <dimension ref="A1:G225"/>
+  <dimension ref="A1:K225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="13.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -527,8 +554,14 @@
       <c r="G1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="3">
+        <v>43840</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -550,8 +583,14 @@
       <c r="G2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -573,8 +612,14 @@
       <c r="G3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -597,7 +642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -620,7 +665,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -643,7 +688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -666,7 +711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -689,7 +734,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -712,7 +757,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -735,7 +780,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -758,7 +803,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -781,7 +826,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -804,7 +849,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -827,7 +872,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -850,7 +895,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -5695,7 +5740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629DD3BE-CA8D-B645-96F3-EDE38C472E9D}">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -5772,7 +5817,7 @@
         <v>17</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:O3" si="0">C10+1</f>
+        <f t="shared" ref="D3:N3" si="0">C10+1</f>
         <v>25</v>
       </c>
       <c r="E3">
@@ -5829,7 +5874,7 @@
         <v>18</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:O4" si="3">D3+1</f>
+        <f t="shared" ref="D4:N4" si="3">D3+1</f>
         <v>26</v>
       </c>
       <c r="E4">
@@ -5886,7 +5931,7 @@
         <v>19</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:O5" si="5">D4+1</f>
+        <f t="shared" ref="D5:N5" si="5">D4+1</f>
         <v>27</v>
       </c>
       <c r="E5">
@@ -5943,7 +5988,7 @@
         <v>20</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:O6" si="7">D5+1</f>
+        <f t="shared" ref="D6:N6" si="7">D5+1</f>
         <v>28</v>
       </c>
       <c r="E6">
@@ -6000,7 +6045,7 @@
         <v>21</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:O7" si="9">D6+1</f>
+        <f t="shared" ref="D7:N7" si="9">D6+1</f>
         <v>29</v>
       </c>
       <c r="E7">
@@ -6057,7 +6102,7 @@
         <v>22</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:O8" si="11">D7+1</f>
+        <f t="shared" ref="D8:N8" si="11">D7+1</f>
         <v>30</v>
       </c>
       <c r="E8">
@@ -6114,7 +6159,7 @@
         <v>23</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:O9" si="13">D8+1</f>
+        <f t="shared" ref="D9:N9" si="13">D8+1</f>
         <v>31</v>
       </c>
       <c r="E9">
@@ -6171,7 +6216,7 @@
         <v>24</v>
       </c>
       <c r="D10">
-        <f t="shared" ref="D10:O10" si="15">D9+1</f>
+        <f t="shared" ref="D10:N10" si="15">D9+1</f>
         <v>32</v>
       </c>
       <c r="E10">
@@ -6282,7 +6327,7 @@
         <v>2</v>
       </c>
       <c r="B13">
-        <f t="shared" ref="B13:O19" si="27">B12+1</f>
+        <f t="shared" ref="B13:N19" si="27">B12+1</f>
         <v>10</v>
       </c>
       <c r="C13">
@@ -6679,6 +6724,10 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;A</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -6687,7 +6736,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:P19"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6752,354 +6801,354 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>1</v>
-      </c>
-      <c r="M4" t="s">
-        <v>1</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
-        <v>1</v>
-      </c>
-      <c r="M5" t="s">
-        <v>1</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
-        <v>1</v>
-      </c>
-      <c r="K6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L6" t="s">
-        <v>1</v>
-      </c>
-      <c r="M6" t="s">
-        <v>1</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" t="s">
-        <v>1</v>
-      </c>
-      <c r="L7" t="s">
-        <v>1</v>
-      </c>
-      <c r="M7" t="s">
-        <v>1</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" t="s">
-        <v>1</v>
-      </c>
-      <c r="K8" t="s">
-        <v>1</v>
-      </c>
-      <c r="L8" t="s">
-        <v>1</v>
-      </c>
-      <c r="M8" t="s">
-        <v>1</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="A8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" t="s">
-        <v>1</v>
-      </c>
-      <c r="K9" t="s">
-        <v>1</v>
-      </c>
-      <c r="L9" t="s">
-        <v>1</v>
-      </c>
-      <c r="M9" t="s">
-        <v>1</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H10" t="s">
-        <v>1</v>
-      </c>
-      <c r="I10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L10" t="s">
-        <v>1</v>
-      </c>
-      <c r="M10" t="s">
-        <v>1</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -7109,354 +7158,354 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" t="s">
-        <v>1</v>
-      </c>
-      <c r="H12" t="s">
-        <v>1</v>
-      </c>
-      <c r="I12" t="s">
-        <v>1</v>
-      </c>
-      <c r="J12" t="s">
-        <v>1</v>
-      </c>
-      <c r="K12" t="s">
-        <v>1</v>
-      </c>
-      <c r="L12" t="s">
-        <v>1</v>
-      </c>
-      <c r="M12" t="s">
-        <v>1</v>
-      </c>
-      <c r="N12" t="s">
+      <c r="A12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N12" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" t="s">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" t="s">
-        <v>1</v>
-      </c>
-      <c r="I13" t="s">
-        <v>1</v>
-      </c>
-      <c r="J13" t="s">
-        <v>1</v>
-      </c>
-      <c r="K13" t="s">
-        <v>1</v>
-      </c>
-      <c r="L13" t="s">
-        <v>1</v>
-      </c>
-      <c r="M13" t="s">
-        <v>1</v>
-      </c>
-      <c r="N13" t="s">
+      <c r="A13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N13" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>1</v>
-      </c>
-      <c r="F14" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>1</v>
-      </c>
-      <c r="H14" t="s">
-        <v>1</v>
-      </c>
-      <c r="I14" t="s">
-        <v>1</v>
-      </c>
-      <c r="J14" t="s">
-        <v>1</v>
-      </c>
-      <c r="K14" t="s">
-        <v>1</v>
-      </c>
-      <c r="L14" t="s">
-        <v>1</v>
-      </c>
-      <c r="M14" t="s">
-        <v>1</v>
-      </c>
-      <c r="N14" t="s">
+      <c r="A14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N14" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>1</v>
-      </c>
-      <c r="H15" t="s">
-        <v>1</v>
-      </c>
-      <c r="I15" t="s">
-        <v>1</v>
-      </c>
-      <c r="J15" t="s">
-        <v>1</v>
-      </c>
-      <c r="K15" t="s">
-        <v>1</v>
-      </c>
-      <c r="L15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N15" t="s">
+      <c r="A15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N15" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>1</v>
-      </c>
-      <c r="H16" t="s">
-        <v>1</v>
-      </c>
-      <c r="I16" t="s">
-        <v>1</v>
-      </c>
-      <c r="J16" t="s">
-        <v>1</v>
-      </c>
-      <c r="K16" t="s">
-        <v>1</v>
-      </c>
-      <c r="L16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M16" t="s">
-        <v>1</v>
-      </c>
-      <c r="N16" t="s">
+      <c r="A16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N16" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
-        <v>1</v>
-      </c>
-      <c r="I17" t="s">
-        <v>1</v>
-      </c>
-      <c r="J17" t="s">
-        <v>1</v>
-      </c>
-      <c r="K17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L17" t="s">
-        <v>1</v>
-      </c>
-      <c r="M17" t="s">
-        <v>1</v>
-      </c>
-      <c r="N17" t="s">
+      <c r="A17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N17" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" t="s">
-        <v>1</v>
-      </c>
-      <c r="I18" t="s">
-        <v>1</v>
-      </c>
-      <c r="J18" t="s">
-        <v>1</v>
-      </c>
-      <c r="K18" t="s">
-        <v>1</v>
-      </c>
-      <c r="L18" t="s">
-        <v>1</v>
-      </c>
-      <c r="M18" t="s">
-        <v>1</v>
-      </c>
-      <c r="N18" t="s">
+      <c r="A18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N18" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
-        <v>1</v>
-      </c>
-      <c r="H19" t="s">
-        <v>1</v>
-      </c>
-      <c r="I19" t="s">
-        <v>1</v>
-      </c>
-      <c r="J19" t="s">
-        <v>1</v>
-      </c>
-      <c r="K19" t="s">
-        <v>1</v>
-      </c>
-      <c r="L19" t="s">
-        <v>1</v>
-      </c>
-      <c r="M19" t="s">
-        <v>1</v>
-      </c>
-      <c r="N19" t="s">
+      <c r="A19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N19" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -7465,10 +7514,10 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
-    <oddHeader>&amp;LExperiment: dist_primary_trans
-&amp;"-,Bold"Germination&amp;Cplants sowed: 12/13/19
-plants inoculated: 12/20/19
-&amp;Rinoculum 3 days old</oddHeader>
+    <oddHeader xml:space="preserve">&amp;LExperiment: dist_primary_trans
+&amp;"-,Bold"&amp;A&amp;C&amp;"System Font,Regular"&amp;10&amp;K000000
+&amp;Rinoculum 3 days old
+</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
@@ -7478,7 +7527,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:P19"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7543,354 +7592,354 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>1</v>
-      </c>
-      <c r="M4" t="s">
-        <v>1</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
-        <v>1</v>
-      </c>
-      <c r="M5" t="s">
-        <v>1</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
-        <v>1</v>
-      </c>
-      <c r="K6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L6" t="s">
-        <v>1</v>
-      </c>
-      <c r="M6" t="s">
-        <v>1</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" t="s">
-        <v>1</v>
-      </c>
-      <c r="L7" t="s">
-        <v>1</v>
-      </c>
-      <c r="M7" t="s">
-        <v>1</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" t="s">
-        <v>1</v>
-      </c>
-      <c r="K8" t="s">
-        <v>1</v>
-      </c>
-      <c r="L8" t="s">
-        <v>1</v>
-      </c>
-      <c r="M8" t="s">
-        <v>1</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="A8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" t="s">
-        <v>1</v>
-      </c>
-      <c r="K9" t="s">
-        <v>1</v>
-      </c>
-      <c r="L9" t="s">
-        <v>1</v>
-      </c>
-      <c r="M9" t="s">
-        <v>1</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H10" t="s">
-        <v>1</v>
-      </c>
-      <c r="I10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L10" t="s">
-        <v>1</v>
-      </c>
-      <c r="M10" t="s">
-        <v>1</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -7900,354 +7949,354 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" t="s">
-        <v>1</v>
-      </c>
-      <c r="H12" t="s">
-        <v>1</v>
-      </c>
-      <c r="I12" t="s">
-        <v>1</v>
-      </c>
-      <c r="J12" t="s">
-        <v>1</v>
-      </c>
-      <c r="K12" t="s">
-        <v>1</v>
-      </c>
-      <c r="L12" t="s">
-        <v>1</v>
-      </c>
-      <c r="M12" t="s">
-        <v>1</v>
-      </c>
-      <c r="N12" t="s">
+      <c r="A12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N12" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" t="s">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" t="s">
-        <v>1</v>
-      </c>
-      <c r="I13" t="s">
-        <v>1</v>
-      </c>
-      <c r="J13" t="s">
-        <v>1</v>
-      </c>
-      <c r="K13" t="s">
-        <v>1</v>
-      </c>
-      <c r="L13" t="s">
-        <v>1</v>
-      </c>
-      <c r="M13" t="s">
-        <v>1</v>
-      </c>
-      <c r="N13" t="s">
+      <c r="A13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N13" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>1</v>
-      </c>
-      <c r="F14" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>1</v>
-      </c>
-      <c r="H14" t="s">
-        <v>1</v>
-      </c>
-      <c r="I14" t="s">
-        <v>1</v>
-      </c>
-      <c r="J14" t="s">
-        <v>1</v>
-      </c>
-      <c r="K14" t="s">
-        <v>1</v>
-      </c>
-      <c r="L14" t="s">
-        <v>1</v>
-      </c>
-      <c r="M14" t="s">
-        <v>1</v>
-      </c>
-      <c r="N14" t="s">
+      <c r="A14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N14" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>1</v>
-      </c>
-      <c r="H15" t="s">
-        <v>1</v>
-      </c>
-      <c r="I15" t="s">
-        <v>1</v>
-      </c>
-      <c r="J15" t="s">
-        <v>1</v>
-      </c>
-      <c r="K15" t="s">
-        <v>1</v>
-      </c>
-      <c r="L15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N15" t="s">
+      <c r="A15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N15" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>1</v>
-      </c>
-      <c r="H16" t="s">
-        <v>1</v>
-      </c>
-      <c r="I16" t="s">
-        <v>1</v>
-      </c>
-      <c r="J16" t="s">
-        <v>1</v>
-      </c>
-      <c r="K16" t="s">
-        <v>1</v>
-      </c>
-      <c r="L16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M16" t="s">
-        <v>1</v>
-      </c>
-      <c r="N16" t="s">
+      <c r="A16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N16" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
-        <v>1</v>
-      </c>
-      <c r="I17" t="s">
-        <v>1</v>
-      </c>
-      <c r="J17" t="s">
-        <v>1</v>
-      </c>
-      <c r="K17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L17" t="s">
-        <v>1</v>
-      </c>
-      <c r="M17" t="s">
-        <v>1</v>
-      </c>
-      <c r="N17" t="s">
+      <c r="A17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N17" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" t="s">
-        <v>1</v>
-      </c>
-      <c r="I18" t="s">
-        <v>1</v>
-      </c>
-      <c r="J18" t="s">
-        <v>1</v>
-      </c>
-      <c r="K18" t="s">
-        <v>1</v>
-      </c>
-      <c r="L18" t="s">
-        <v>1</v>
-      </c>
-      <c r="M18" t="s">
-        <v>1</v>
-      </c>
-      <c r="N18" t="s">
+      <c r="A18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N18" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
-        <v>1</v>
-      </c>
-      <c r="H19" t="s">
-        <v>1</v>
-      </c>
-      <c r="I19" t="s">
-        <v>1</v>
-      </c>
-      <c r="J19" t="s">
-        <v>1</v>
-      </c>
-      <c r="K19" t="s">
-        <v>1</v>
-      </c>
-      <c r="L19" t="s">
-        <v>1</v>
-      </c>
-      <c r="M19" t="s">
-        <v>1</v>
-      </c>
-      <c r="N19" t="s">
+      <c r="A19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N19" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -8257,9 +8306,7 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
     <oddHeader>&amp;LExperiment: dist_primary_trans
-&amp;"-,Bold"Germination&amp;Cplants sowed: 12/13/19
-plants inoculated: 12/20/19
-&amp;Rinoculum 3 days old</oddHeader>
+&amp;"-,Bold"&amp;A&amp;Rinoculum 3 days old</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
@@ -8268,8 +8315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29BDB138-3322-3245-9BF4-3564AACD8190}">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:P19"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9080,8 +9127,7 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Calibri,Regular"&amp;K000000Experiment: Dist_primary_trans
-&amp;"Calibri,Bold"Infection&amp;C&amp;"Calibri,Regular"&amp;K000000plants sowed: 12/13/19
-plants inoculated: 12/20/19&amp;R&amp;"Calibri,Regular"&amp;K000000inoculum 3 days old</oddHeader>
+&amp;"Calibri,Bold"&amp;A&amp;R&amp;"Calibri,Regular"&amp;K000000inoculum 3 days old</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
@@ -9090,7 +9136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0F7117-499C-0D4C-BC11-A5B5F7CEC9FD}">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
@@ -9902,8 +9948,7 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Calibri,Regular"&amp;K000000Experiment: Dist_primary_trans
-&amp;"Calibri,Bold"Infection&amp;C&amp;"Calibri,Regular"&amp;K000000plants sowed: 12/13/19
-plants inoculated: 12/20/19&amp;R&amp;"Calibri,Regular"&amp;K000000inoculum 3 days old</oddHeader>
+&amp;"Calibri,Bold"&amp;A&amp;R&amp;"Calibri,Regular"&amp;K000000inoculum 3 days old</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>